<commit_message>
able to generate gap scores
</commit_message>
<xml_diff>
--- a/data/formation_template.xlsx
+++ b/data/formation_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garre\Documents\GitHub\javascript-football-simulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586F5543-B122-428F-9662-0ABF3EDE52C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4F3CFA-8760-4FA8-9C1A-F9E0A83F90B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="12" xr2:uid="{F71E664A-AF11-416A-99DD-E04303549019}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F71E664A-AF11-416A-99DD-E04303549019}"/>
   </bookViews>
   <sheets>
     <sheet name="4-3" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="44">
   <si>
     <t>Deep</t>
   </si>
@@ -147,6 +147,36 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>C+</t>
+  </si>
+  <si>
+    <t>D+</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>C-</t>
+  </si>
+  <si>
+    <t>D-</t>
+  </si>
+  <si>
+    <t>Contain+</t>
+  </si>
+  <si>
+    <t>Contain-</t>
   </si>
 </sst>
 </file>
@@ -410,439 +440,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="74" name="Straight Arrow Connector 73">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{979F5A5A-26FF-46AC-A1EA-2D7E86EC3975}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="4267200" y="2049780"/>
-          <a:ext cx="175260" cy="182880"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="76" name="Straight Arrow Connector 75">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{771DDC9A-C571-428F-A2BA-06636C68E63E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4610100" y="2263140"/>
-          <a:ext cx="213360" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>243840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="80" name="Straight Arrow Connector 79">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1956E56D-3C61-427F-AD85-D4EF7FDF3C4F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5181600" y="2072640"/>
-          <a:ext cx="137160" cy="121920"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="82" name="Straight Arrow Connector 81">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1814B8B3-4591-4FFE-91A8-93D26136DAF8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3055620" y="2042160"/>
-          <a:ext cx="152400" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="84" name="Straight Arrow Connector 83">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACF393E2-776F-4919-AD0C-5EA8E1E6B129}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3985260" y="2171700"/>
-          <a:ext cx="541020" cy="83820"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>220980</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="86" name="Straight Arrow Connector 85">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{283D7F28-39E6-4F3C-97AE-CF4686E6E490}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5791200" y="2049780"/>
-          <a:ext cx="167640" cy="182880"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>274320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="88" name="Straight Arrow Connector 87">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9BFCE96-6717-466F-8F34-B9F698599926}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="6332220" y="1493520"/>
-          <a:ext cx="7620" cy="708660"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>220980</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="91" name="Straight Arrow Connector 90">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21A18FBC-516F-4327-B85B-29FC1A892A57}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="4503420" y="1440180"/>
-          <a:ext cx="22860" cy="723900"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>220980</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
         <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5654CFFF-3C6E-4CD3-A2FE-67F14B03A67C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74B6960A-F5C9-437B-9E52-6415A8EED6E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -895,7 +496,7 @@
         <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3208063-4B6B-431B-B735-A9089B955D60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7025A8B-2599-40A0-ABF7-51ED508254BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -948,7 +549,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1BAFA0B-B274-44E8-BF2B-B7A8ADFEB4A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3D3453-DEA8-4064-9027-4629FE452581}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1001,7 +602,7 @@
         <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2493139-B0AB-4FF0-9FE0-EC4807107392}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6142DAC-8014-42B3-8902-F1713D9D2C53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1054,7 +655,7 @@
         <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92928610-EAEC-439D-8A9A-BA52C098A99F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7693C145-CF6A-4F54-AF11-002D400845FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1107,7 +708,7 @@
         <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B7E942-166F-497E-999B-9AC34BE9D316}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F80CC152-C4D8-4991-8856-C317778AE29B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1160,7 +761,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{131D571D-654A-47E0-978C-26E1C88CF54C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DC167C-39EB-49D7-98C9-D648AFC25FCA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1213,7 +814,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2F386C4-432B-4F0D-9B64-E6513BAD0C75}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E77FCA4-60AE-45AF-8EEB-E0D0A64C191B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1251,7 +852,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1627,7 +1228,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2060,435 +1661,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>220980</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74B6960A-F5C9-437B-9E52-6415A8EED6E2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="4267200" y="2049780"/>
-          <a:ext cx="175260" cy="182880"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7025A8B-2599-40A0-ABF7-51ED508254BC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4610100" y="2263140"/>
-          <a:ext cx="213360" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>236220</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3D3453-DEA8-4064-9027-4629FE452581}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="4572000" y="1455420"/>
-          <a:ext cx="251460" cy="777240"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>243840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6142DAC-8014-42B3-8902-F1713D9D2C53}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5181600" y="2072640"/>
-          <a:ext cx="137160" cy="121920"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7693C145-CF6A-4F54-AF11-002D400845FA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3055620" y="2042160"/>
-          <a:ext cx="152400" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>259080</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F80CC152-C4D8-4991-8856-C317778AE29B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3680460" y="1478280"/>
-          <a:ext cx="190500" cy="716280"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>220980</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DC167C-39EB-49D7-98C9-D648AFC25FCA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5791200" y="1440180"/>
-          <a:ext cx="205740" cy="792480"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>220980</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E77FCA4-60AE-45AF-8EEB-E0D0A64C191B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6339840" y="2049780"/>
-          <a:ext cx="0" cy="152400"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>99060</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -2861,7 +2033,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3237,7 +2409,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3613,7 +2785,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4042,7 +3214,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4418,7 +3590,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4847,7 +4019,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5248,6 +4420,435 @@
         <a:xfrm flipV="1">
           <a:off x="2948940" y="1767840"/>
           <a:ext cx="0" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5654CFFF-3C6E-4CD3-A2FE-67F14B03A67C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4267200" y="2049780"/>
+          <a:ext cx="175260" cy="182880"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3208063-4B6B-431B-B735-A9089B955D60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4610100" y="2263140"/>
+          <a:ext cx="213360" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>236220</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1BAFA0B-B274-44E8-BF2B-B7A8ADFEB4A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4572000" y="1455420"/>
+          <a:ext cx="251460" cy="777240"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>243840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2493139-B0AB-4FF0-9FE0-EC4807107392}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5181600" y="2072640"/>
+          <a:ext cx="137160" cy="121920"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92928610-EAEC-439D-8A9A-BA52C098A99F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3055620" y="2042160"/>
+          <a:ext cx="152400" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B7E942-166F-497E-999B-9AC34BE9D316}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3680460" y="1478280"/>
+          <a:ext cx="190500" cy="716280"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{131D571D-654A-47E0-978C-26E1C88CF54C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5791200" y="1440180"/>
+          <a:ext cx="205740" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2F386C4-432B-4F0D-9B64-E6513BAD0C75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6339840" y="2049780"/>
+          <a:ext cx="0" cy="152400"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5575,8 +5176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E84AF4-DBED-485F-BEF7-3FC0799A6865}">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5751,9 +5352,7 @@
       <c r="G4" s="14"/>
       <c r="H4" s="9"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -5763,9 +5362,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
-      <c r="T4" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="14"/>
       <c r="W4" s="9"/>
@@ -5787,24 +5384,18 @@
       <c r="G5" s="14"/>
       <c r="H5" s="9"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="U5" s="5"/>
       <c r="V5" s="14"/>
       <c r="W5" s="9"/>
       <c r="X5" s="5"/>
@@ -5851,41 +5442,49 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="10"/>
       <c r="F7" s="8"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="10"/>
+      <c r="H7" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="L7" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="M7" s="8"/>
       <c r="N7" s="8" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+      <c r="P7" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="S7" s="8"/>
       <c r="T7" s="8" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="U7" s="8"/>
-      <c r="V7" s="15"/>
+      <c r="V7" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="W7" s="10"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="15"/>
       <c r="Z7" s="10"/>
       <c r="AA7" s="8" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AB7" s="8"/>
     </row>
@@ -5902,7 +5501,9 @@
       <c r="F8" s="7"/>
       <c r="G8" s="16"/>
       <c r="H8" s="11"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7" t="s">
         <v>9</v>
@@ -5988,9 +5589,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
-      <c r="O10" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
@@ -6080,7 +5679,6 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7627,7 +7225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24206657-E129-4FB6-9CB3-5132F2076CC3}">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
estimate where block occurs using 1D math
</commit_message>
<xml_diff>
--- a/data/formation_template.xlsx
+++ b/data/formation_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garre\Documents\GitHub\javascript-football-simulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4F3CFA-8760-4FA8-9C1A-F9E0A83F90B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2574DA-B88F-4BB7-97C2-446823D1452C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F71E664A-AF11-416A-99DD-E04303549019}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F71E664A-AF11-416A-99DD-E04303549019}"/>
   </bookViews>
   <sheets>
     <sheet name="4-3" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="46">
   <si>
     <t>Deep</t>
   </si>
@@ -173,10 +173,16 @@
     <t>D-</t>
   </si>
   <si>
-    <t>Contain+</t>
+    <t>E-</t>
   </si>
   <si>
-    <t>Contain-</t>
+    <t>E+</t>
+  </si>
+  <si>
+    <t>Between Hashes</t>
+  </si>
+  <si>
+    <t>Between Numbers</t>
   </si>
 </sst>
 </file>
@@ -206,7 +212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -346,11 +352,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,6 +419,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5174,10 +5192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E84AF4-DBED-485F-BEF7-3FC0799A6865}">
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2:AC12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5198,7 +5216,7 @@
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -5441,11 +5459,11 @@
         <v>4</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F7" s="8"/>
       <c r="G7" s="15"/>
       <c r="H7" s="10" t="s">
@@ -5481,11 +5499,11 @@
       </c>
       <c r="W7" s="10"/>
       <c r="X7" s="8"/>
-      <c r="Y7" s="15"/>
+      <c r="Y7" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="Z7" s="10"/>
-      <c r="AA7" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="AA7" s="8"/>
       <c r="AB7" s="8"/>
     </row>
     <row r="8" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -5670,8 +5688,46 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
     </row>
+    <row r="13" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="E13:Y13"/>
+    <mergeCell ref="Z13:AB13"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="H1:V1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="Z1:AB1"/>

</xml_diff>

<commit_message>
updated rushing sim to include pvp matchups
</commit_message>
<xml_diff>
--- a/data/formation_template.xlsx
+++ b/data/formation_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a675523a8f6b542f/Documents/GitHub/javascript-football-simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4F3F115-5516-46C7-9EA5-CB7363D119A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{A4F3F115-5516-46C7-9EA5-CB7363D119A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D9FDFD35-E242-4203-A33C-83D90937A835}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F71E664A-AF11-416A-99DD-E04303549019}"/>
   </bookViews>
@@ -5562,7 +5562,7 @@
   <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5908,9 +5908,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="16"/>
       <c r="I8" s="23"/>
-      <c r="J8" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="J8" s="7"/>
       <c r="K8" s="26"/>
       <c r="L8" s="7" t="s">
         <v>9</v>
@@ -5954,7 +5952,9 @@
       <c r="E9" s="27"/>
       <c r="F9" s="12"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="17"/>
+      <c r="H9" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="I9" s="21"/>
       <c r="J9" s="6"/>
       <c r="K9" s="24"/>
@@ -5976,9 +5976,7 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="17"/>
       <c r="AA9" s="21"/>
-      <c r="AB9" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="AB9" s="17"/>
       <c r="AC9" s="12"/>
       <c r="AD9" s="38"/>
     </row>
@@ -6000,7 +5998,9 @@
       <c r="M10" s="24"/>
       <c r="N10" s="6"/>
       <c r="O10" s="24"/>
-      <c r="P10" s="6"/>
+      <c r="P10" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="Q10" s="24"/>
       <c r="R10" s="6"/>
       <c r="S10" s="24"/>

</xml_diff>

<commit_message>
pseudo physics update for run sim
</commit_message>
<xml_diff>
--- a/data/formation_template.xlsx
+++ b/data/formation_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a675523a8f6b542f/Documents/GitHub/javascript-football-simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{A4F3F115-5516-46C7-9EA5-CB7363D119A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D9FDFD35-E242-4203-A33C-83D90937A835}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{A4F3F115-5516-46C7-9EA5-CB7363D119A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1BF9F503-5EC3-4D9C-819B-9B469C3B0576}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F71E664A-AF11-416A-99DD-E04303549019}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="61">
   <si>
     <t>Deep</t>
   </si>
@@ -211,6 +211,27 @@
   <si>
     <t>Numbers</t>
   </si>
+  <si>
+    <t>u1</t>
+  </si>
+  <si>
+    <t>u2</t>
+  </si>
+  <si>
+    <t>u3</t>
+  </si>
+  <si>
+    <t>u4</t>
+  </si>
+  <si>
+    <t>u3/4</t>
+  </si>
+  <si>
+    <t>u5</t>
+  </si>
+  <si>
+    <t>u6</t>
+  </si>
 </sst>
 </file>
 
@@ -233,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,8 +285,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -545,11 +572,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -729,6 +819,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5562,7 +5676,7 @@
   <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5776,35 +5890,49 @@
       <c r="A5" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="47"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="35"/>
+      <c r="B5" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
+      <c r="V5" s="62"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y5" s="62"/>
+      <c r="Z5" s="62"/>
+      <c r="AA5" s="63"/>
+      <c r="AB5" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC5" s="62"/>
+      <c r="AD5" s="68"/>
     </row>
     <row r="6" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
@@ -6121,7 +6249,13 @@
       <c r="N16" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="Q5:W5"/>
     <mergeCell ref="I1:W1"/>
     <mergeCell ref="X1:Z1"/>
     <mergeCell ref="F1:H1"/>

</xml_diff>

<commit_message>
refactored and cleaned up defender zone assignment
</commit_message>
<xml_diff>
--- a/data/formation_template.xlsx
+++ b/data/formation_template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a675523a8f6b542f/Documents/GitHub/javascript-football-simulation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfoster\OneDrive\Documents\GitHub\javascript-football-simulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{A4F3F115-5516-46C7-9EA5-CB7363D119A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1BF9F503-5EC3-4D9C-819B-9B469C3B0576}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F71E664A-AF11-416A-99DD-E04303549019}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="4-3" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
     <sheet name="Blocks" sheetId="16" r:id="rId15"/>
     <sheet name="Tackles" sheetId="17" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="54">
   <si>
     <t>Deep</t>
   </si>
@@ -211,32 +210,11 @@
   <si>
     <t>Numbers</t>
   </si>
-  <si>
-    <t>u1</t>
-  </si>
-  <si>
-    <t>u2</t>
-  </si>
-  <si>
-    <t>u3</t>
-  </si>
-  <si>
-    <t>u4</t>
-  </si>
-  <si>
-    <t>u3/4</t>
-  </si>
-  <si>
-    <t>u5</t>
-  </si>
-  <si>
-    <t>u6</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -254,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,14 +263,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="28">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -442,11 +414,31 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="mediumDashed">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -457,7 +449,7 @@
       <right style="mediumDashed">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -465,18 +457,40 @@
     </border>
     <border>
       <left/>
-      <right style="thick">
+      <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thick">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -491,7 +505,48 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thick">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -506,131 +561,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="mediumDashed">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -639,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -731,53 +668,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -800,49 +692,70 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5672,11 +5585,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E84AF4-DBED-485F-BEF7-3FC0799A6865}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5688,355 +5601,346 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="58" t="s">
+      <c r="A1" s="31"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="55" t="s">
+      <c r="E1" s="46"/>
+      <c r="F1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="54" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55" t="s">
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="58" t="s">
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="45"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="49"/>
     </row>
     <row r="2" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="18">
+      <c r="A2" s="31"/>
+      <c r="B2" s="50">
         <v>-25</v>
       </c>
       <c r="C2" s="13">
         <v>-22</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="51">
         <v>-19</v>
       </c>
       <c r="E2" s="13">
         <v>-16</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="51">
         <v>-13</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="51">
         <v>-11</v>
       </c>
       <c r="H2" s="13">
         <v>-9</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="51">
         <v>-7</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="51">
         <v>-6</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="51">
         <v>-5</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="51">
         <v>-4</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="51">
         <v>-3</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="51">
         <v>-2</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="51">
         <v>-1</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="51">
         <v>0</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="51">
         <v>1</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="51">
         <v>2</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="51">
         <v>3</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="51">
         <v>4</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="51">
         <v>5</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="51">
         <v>6</v>
       </c>
       <c r="W2" s="13">
         <v>7</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="51">
         <v>9</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="51">
         <v>11</v>
       </c>
       <c r="Z2" s="13">
         <v>13</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="51">
         <v>16</v>
       </c>
       <c r="AB2" s="13">
         <v>19</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2" s="51">
         <v>22</v>
       </c>
-      <c r="AD2" s="46">
+      <c r="AD2" s="52">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="14"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="49"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="9"/>
       <c r="G3" s="5"/>
       <c r="H3" s="14"/>
-      <c r="I3" s="47"/>
+      <c r="I3" s="32"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="51"/>
+      <c r="K3" s="36"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="51"/>
+      <c r="M3" s="36"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="51"/>
+      <c r="O3" s="36"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="51"/>
+      <c r="Q3" s="36"/>
       <c r="R3" s="5"/>
-      <c r="S3" s="51"/>
+      <c r="S3" s="36"/>
       <c r="T3" s="5"/>
-      <c r="U3" s="51"/>
+      <c r="U3" s="36"/>
       <c r="V3" s="5"/>
-      <c r="W3" s="49"/>
+      <c r="W3" s="34"/>
       <c r="X3" s="9"/>
       <c r="Y3" s="5"/>
       <c r="Z3" s="14"/>
-      <c r="AA3" s="47"/>
+      <c r="AA3" s="32"/>
       <c r="AB3" s="14"/>
       <c r="AC3" s="9"/>
-      <c r="AD3" s="35"/>
+      <c r="AD3" s="54"/>
     </row>
     <row r="4" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="14"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="49"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="9"/>
       <c r="G4" s="5"/>
       <c r="H4" s="14"/>
-      <c r="I4" s="47"/>
+      <c r="I4" s="32"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="51"/>
+      <c r="K4" s="36"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="51"/>
+      <c r="M4" s="36"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="51"/>
+      <c r="O4" s="36"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="51"/>
+      <c r="Q4" s="36"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="51"/>
+      <c r="S4" s="36"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="51"/>
+      <c r="U4" s="36"/>
       <c r="V4" s="5"/>
-      <c r="W4" s="49"/>
+      <c r="W4" s="34"/>
       <c r="X4" s="9"/>
       <c r="Y4" s="5"/>
       <c r="Z4" s="14"/>
-      <c r="AA4" s="47"/>
+      <c r="AA4" s="32"/>
       <c r="AB4" s="14"/>
       <c r="AC4" s="9"/>
-      <c r="AD4" s="35"/>
+      <c r="AD4" s="54"/>
     </row>
     <row r="5" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="67" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q5" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="R5" s="62"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="62"/>
-      <c r="U5" s="62"/>
-      <c r="V5" s="62"/>
-      <c r="W5" s="65"/>
-      <c r="X5" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y5" s="62"/>
-      <c r="Z5" s="62"/>
-      <c r="AA5" s="63"/>
-      <c r="AB5" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC5" s="62"/>
-      <c r="AD5" s="68"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="36"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="5"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="36"/>
+      <c r="V5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="W5" s="34"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="54"/>
     </row>
     <row r="6" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="14"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="49"/>
+      <c r="E6" s="34" t="s">
+        <v>26</v>
+      </c>
       <c r="F6" s="9"/>
       <c r="G6" s="5"/>
       <c r="H6" s="14"/>
-      <c r="I6" s="47"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="51"/>
+      <c r="K6" s="36"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="51"/>
+      <c r="M6" s="36"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="51"/>
+      <c r="O6" s="36"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="51"/>
+      <c r="Q6" s="36"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="51"/>
+      <c r="S6" s="36"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="51"/>
+      <c r="U6" s="36"/>
       <c r="V6" s="5"/>
-      <c r="W6" s="49"/>
+      <c r="W6" s="34"/>
       <c r="X6" s="9"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="14"/>
-      <c r="AA6" s="47"/>
+      <c r="AA6" s="32" t="s">
+        <v>26</v>
+      </c>
       <c r="AB6" s="14"/>
       <c r="AC6" s="9"/>
-      <c r="AD6" s="35"/>
-    </row>
-    <row r="7" spans="1:31" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="AD6" s="54"/>
+    </row>
+    <row r="7" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" s="8"/>
-      <c r="S7" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="T7" s="8"/>
-      <c r="U7" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="V7" s="8"/>
-      <c r="W7" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB7" s="15"/>
-      <c r="AC7" s="10"/>
-      <c r="AD7" s="36"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="32"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="54"/>
     </row>
     <row r="8" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="16"/>
       <c r="D8" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="11"/>
       <c r="G8" s="7"/>
       <c r="H8" s="16"/>
       <c r="I8" s="23"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="K8" s="26"/>
       <c r="L8" s="7" t="s">
         <v>9</v>
@@ -6068,21 +5972,19 @@
       <c r="AA8" s="23"/>
       <c r="AB8" s="16"/>
       <c r="AC8" s="11"/>
-      <c r="AD8" s="37"/>
+      <c r="AD8" s="56"/>
     </row>
     <row r="9" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="17"/>
       <c r="D9" s="12"/>
       <c r="E9" s="27"/>
       <c r="F9" s="12"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="H9" s="17"/>
       <c r="I9" s="21"/>
       <c r="J9" s="6"/>
       <c r="K9" s="24"/>
@@ -6090,9 +5992,7 @@
       <c r="M9" s="24"/>
       <c r="N9" s="6"/>
       <c r="O9" s="24"/>
-      <c r="P9" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="P9" s="6"/>
       <c r="Q9" s="24"/>
       <c r="R9" s="6"/>
       <c r="S9" s="24"/>
@@ -6104,15 +6004,17 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="17"/>
       <c r="AA9" s="21"/>
-      <c r="AB9" s="17"/>
+      <c r="AB9" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="AC9" s="12"/>
-      <c r="AD9" s="38"/>
+      <c r="AD9" s="58"/>
     </row>
     <row r="10" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="17"/>
       <c r="D10" s="12"/>
       <c r="E10" s="27"/>
@@ -6126,9 +6028,6 @@
       <c r="M10" s="24"/>
       <c r="N10" s="6"/>
       <c r="O10" s="24"/>
-      <c r="P10" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="Q10" s="24"/>
       <c r="R10" s="6"/>
       <c r="S10" s="24"/>
@@ -6142,13 +6041,13 @@
       <c r="AA10" s="21"/>
       <c r="AB10" s="17"/>
       <c r="AC10" s="12"/>
-      <c r="AD10" s="38"/>
+      <c r="AD10" s="58"/>
     </row>
     <row r="11" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="17"/>
       <c r="D11" s="12"/>
       <c r="E11" s="27"/>
@@ -6163,10 +6062,12 @@
       <c r="N11" s="6"/>
       <c r="O11" s="24"/>
       <c r="P11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="6"/>
       <c r="S11" s="24"/>
       <c r="T11" s="6"/>
       <c r="U11" s="24"/>
@@ -6178,13 +6079,13 @@
       <c r="AA11" s="21"/>
       <c r="AB11" s="17"/>
       <c r="AC11" s="12"/>
-      <c r="AD11" s="38"/>
+      <c r="AD11" s="58"/>
     </row>
     <row r="12" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="42"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="17"/>
       <c r="D12" s="12"/>
       <c r="E12" s="27"/>
@@ -6212,50 +6113,65 @@
       <c r="AA12" s="21"/>
       <c r="AB12" s="17"/>
       <c r="AC12" s="12"/>
-      <c r="AD12" s="43"/>
-      <c r="AE12" s="44"/>
-    </row>
-    <row r="13" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-      <c r="U13" s="39"/>
-      <c r="V13" s="39"/>
-      <c r="W13" s="39"/>
-      <c r="X13" s="39"/>
-      <c r="Y13" s="39"/>
-      <c r="Z13" s="39"/>
-      <c r="AA13" s="39"/>
-      <c r="AB13" s="39"/>
-      <c r="AC13" s="39"/>
-      <c r="AD13" s="40"/>
+      <c r="AD12" s="58"/>
+      <c r="AE12" s="39"/>
+    </row>
+    <row r="13" spans="1:31" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="59"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" s="8"/>
+      <c r="O13" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="R13" s="8"/>
+      <c r="S13" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="T13" s="8"/>
+      <c r="U13" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="V13" s="8"/>
+      <c r="W13" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="60"/>
     </row>
     <row r="16" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N16" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="Q5:W5"/>
+  <mergeCells count="5">
     <mergeCell ref="I1:W1"/>
     <mergeCell ref="X1:Z1"/>
     <mergeCell ref="F1:H1"/>
@@ -6267,7 +6183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032F2266-89CA-40BB-AC96-303DA8BB7C02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6281,43 +6197,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -6780,7 +6696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032B13C6-755B-4DBC-BEAA-9AC4EC590696}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6794,43 +6710,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -7293,7 +7209,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD018F98-5890-45AB-96DD-08C4926B1B05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7307,43 +7223,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -7806,7 +7722,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24206657-E129-4FB6-9CB3-5132F2076CC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7820,43 +7736,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -8319,7 +8235,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3ACDA26-D9EC-4A76-A666-04E0D8EBBC4E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8333,43 +8249,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -8819,39 +8735,39 @@
       <c r="AB12" s="6"/>
     </row>
     <row r="13" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="60" t="s">
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="60"/>
-      <c r="V13" s="60"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="54" t="s">
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA13" s="54"/>
-      <c r="AB13" s="54"/>
+      <c r="AA13" s="40"/>
+      <c r="AB13" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -8869,7 +8785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B282A339-F35E-4E22-BB37-8D821DA2DA4D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8883,43 +8799,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -9369,39 +9285,39 @@
       <c r="AB12" s="6"/>
     </row>
     <row r="13" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="60" t="s">
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="60"/>
-      <c r="V13" s="60"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="54" t="s">
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA13" s="54"/>
-      <c r="AB13" s="54"/>
+      <c r="AA13" s="40"/>
+      <c r="AB13" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -9419,7 +9335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0F7A44-D828-4D26-9912-FE5F4B0952E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9433,43 +9349,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -9899,39 +9815,39 @@
       <c r="AB12" s="6"/>
     </row>
     <row r="13" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="60" t="s">
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="60"/>
-      <c r="V13" s="60"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="54" t="s">
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA13" s="54"/>
-      <c r="AB13" s="54"/>
+      <c r="AA13" s="40"/>
+      <c r="AB13" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -9950,7 +9866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A7A1CD-08B1-4332-BE9C-41E398AA5AFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9964,43 +9880,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -10400,7 +10316,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="53" t="s">
+      <c r="O11" s="38" t="s">
         <v>12</v>
       </c>
       <c r="P11" s="6"/>
@@ -10463,7 +10379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F065C51-F8B3-40E1-B370-5F32DBBA278A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10477,43 +10393,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -10976,7 +10892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20824D77-775F-40EC-9339-E1614558ABFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10990,43 +10906,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -11489,7 +11405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BD385B-09A8-4A35-967A-3CC52421623B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11503,43 +11419,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -12002,7 +11918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E39EF2-9D26-43AE-9939-2DFCF9EEB394}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12016,43 +11932,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -12515,7 +12431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F905519A-A288-4976-B87C-0B2942775711}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12529,43 +12445,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -13028,7 +12944,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1446559-B5F2-49E4-AED3-5963B37FB213}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13042,43 +12958,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
@@ -13541,7 +13457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5350B2-4269-4BD6-AD1C-26FC5256B150}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13555,43 +13471,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
     </row>
     <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2">

</xml_diff>